<commit_message>
Zobrazení akcí bez validních učitelů
Bombátor nyní zobrazí akce bez učitelů. Ten postup je trochu iffy, ale minimálně teoreticky by to fungovat mělo, a co jsem koukal tak i výsledky dávaj smysl.
Teď by tam mělo být vše, co je nutné k zobrazení prvního legit výsledku. Yaaaay.
</commit_message>
<xml_diff>
--- a/results/chybi_cvicici.xlsx
+++ b/results/chybi_cvicici.xlsx
@@ -250,8 +250,8 @@
     <t>TYD/SEM</t>
   </si>
   <si>
-    <t>Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe).
-Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia.
+    <t>Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe)._x000D_
+Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia._x000D_
 Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů.</t>
   </si>
   <si>
@@ -264,9 +264,9 @@
     <t>Zápočet je udělen základě potvrzení o vykonané praxi vydané poskytovatelem praxe (jeho součástí je zhodnocení pověřenou osobou) a zprávy praktikanta o průběhu odborné praxe</t>
   </si>
   <si>
-    <t xml:space="preserve">Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe).
-Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia.
-Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů. 
+    <t xml:space="preserve">Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe)._x000D_
+Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia._x000D_
+Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů. _x000D_
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Spravené kontroly hodin bez validních učitelů
Teď by ty výsledky mohly bejt v pohodě
</commit_message>
<xml_diff>
--- a/results/chybi_cvicici.xlsx
+++ b/results/chybi_cvicici.xlsx
@@ -250,8 +250,8 @@
     <t>TYD/SEM</t>
   </si>
   <si>
-    <t>Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe)._x000D_
-Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia._x000D_
+    <t>Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe).
+Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia.
 Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů.</t>
   </si>
   <si>
@@ -264,9 +264,9 @@
     <t>Zápočet je udělen základě potvrzení o vykonané praxi vydané poskytovatelem praxe (jeho součástí je zhodnocení pověřenou osobou) a zprávy praktikanta o průběhu odborné praxe</t>
   </si>
   <si>
-    <t xml:space="preserve">Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe)._x000D_
-Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia._x000D_
-Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů. _x000D_
+    <t xml:space="preserve">Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe).
+Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia.
+Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů. 
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Tabulky fakulty: Pokus o načítání
Problém: Chyba v castění
Řešení jsou bandaid fixes a všechno je to na hovno

bordel.wav
</commit_message>
<xml_diff>
--- a/results/chybi_cvicici.xlsx
+++ b/results/chybi_cvicici.xlsx
@@ -250,8 +250,8 @@
     <t>TYD/SEM</t>
   </si>
   <si>
-    <t>Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe).
-Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia.
+    <t>Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe)._x000D_
+Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia._x000D_
 Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů.</t>
   </si>
   <si>
@@ -264,9 +264,9 @@
     <t>Zápočet je udělen základě potvrzení o vykonané praxi vydané poskytovatelem praxe (jeho součástí je zhodnocení pověřenou osobou) a zprávy praktikanta o průběhu odborné praxe</t>
   </si>
   <si>
-    <t xml:space="preserve">Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe).
-Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia.
-Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů. 
+    <t xml:space="preserve">Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe)._x000D_
+Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia._x000D_
+Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů. _x000D_
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Ignore jsem ve špatný větvi
</commit_message>
<xml_diff>
--- a/results/chybi_cvicici.xlsx
+++ b/results/chybi_cvicici.xlsx
@@ -250,8 +250,8 @@
     <t>TYD/SEM</t>
   </si>
   <si>
-    <t>Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe).
-Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia.
+    <t>Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe)._x000D_
+Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia._x000D_
 Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů.</t>
   </si>
   <si>
@@ -264,9 +264,9 @@
     <t>Zápočet je udělen základě potvrzení o vykonané praxi vydané poskytovatelem praxe (jeho součástí je zhodnocení pověřenou osobou) a zprávy praktikanta o průběhu odborné praxe</t>
   </si>
   <si>
-    <t xml:space="preserve">Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe).
-Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia.
-Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů. 
+    <t xml:space="preserve">Odborná praxe je přednostně uskutečňována na pracovištích, se kterými katedra dlouhodobě spolupracuje, a to v rámci společných projektů (včetně projektů smluvního výzkumu). Praxe může být provázána s projektovým seminářem, který probíhá v obou semestrech posledního ročníku (v rámci projektového semináře skupina studentů může spolupracovat na projektu, jehož část je připravována v rámci praxe)._x000D_
+Odborná praxe může být realizována až po skončení výuky v letním semestru druhého roku studia._x000D_
+Minimální rozsah odborné praxe v týdnech je 12, v hodinách 480. Základní model realizace odborné praxe je 4 dny týdně po 8 hodinách po dobu 15 týdnů v řadě, přičemž prvních 13 týdnů je zařazeno ve výukových týdnech pátého semestru (v něm je výuka naplánována pouze na jeden volný den týdne, a je proto mnohdy bloková) a zbývající 2 týdny v navazujícím zkouškovém období. Přípustné je i jiné rozložení odborné praxe, které zachová požadovaný minimální rozsah a nepřekrývá se s ostatní přímou výukou. Další podporovaný model odborné praxe má formu zahraniční pracovní stáže v rámci projektu Erasmus+ nebo jiného přeshraničního projektu v minimálním rozsahu 12 týdnů. _x000D_
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Generování ok předmětů a základ pro xlsx -> csv
</commit_message>
<xml_diff>
--- a/results/chybi_cvicici.xlsx
+++ b/results/chybi_cvicici.xlsx
@@ -529,12 +529,12 @@
     <t>Reg. geography of Northwestern Bohemia</t>
   </si>
   <si>
+    <t>Regional geography of the Czech Republic</t>
+  </si>
+  <si>
     <t>Sociobiology</t>
   </si>
   <si>
-    <t>Regional geography of the Czech Republic</t>
-  </si>
-  <si>
     <t>General Zoology</t>
   </si>
   <si>
@@ -580,21 +580,21 @@
     <t>Seminář z analytické chemie</t>
   </si>
   <si>
+    <t>PVK - Elektronika II</t>
+  </si>
+  <si>
     <t>PVK - Mykologie</t>
   </si>
   <si>
-    <t>PVK - Elektronika II</t>
-  </si>
-  <si>
     <t>Instrumentální analýza</t>
   </si>
   <si>
+    <t>PVK-Kvantová fyzika II</t>
+  </si>
+  <si>
     <t>Evoluční biologie</t>
   </si>
   <si>
-    <t>PVK-Kvantová fyzika II</t>
-  </si>
-  <si>
     <t>PVK - Mikroprocesorová technika</t>
   </si>
   <si>
@@ -625,12 +625,12 @@
     <t>Přednášky učitelů z praxe</t>
   </si>
   <si>
+    <t>Diplomová práce III</t>
+  </si>
+  <si>
     <t>Matematický seminář</t>
   </si>
   <si>
-    <t>Diplomová práce III</t>
-  </si>
-  <si>
     <t>Metody sledování zvířat</t>
   </si>
   <si>
@@ -703,10 +703,10 @@
     <t>Informační technologie v biologických vědách II</t>
   </si>
   <si>
+    <t>Elektronika II</t>
+  </si>
+  <si>
     <t>Mykologie</t>
-  </si>
-  <si>
-    <t>Elektronika II</t>
   </si>
   <si>
     <t>Mikroprocesorová technika</t>
@@ -1624,10 +1624,10 @@
     <t>The course focuses on selected geographical aspects of NW Bohemia, mainly as follows: (a) location and geodiversity - evolution of natural environment, landscape types, (b) development of settlement, history and recent demographical trends, (c) economic significance of the region, (d) cross-border relations with Germany (Saxony), (e) environmental problems and (f) regional development issues. Students are attending consultations, where they get tasks and discussion questions for the above mentioned issues, and concurrently they work on a project covering these issues.</t>
   </si>
   <si>
+    <t>The course focuses on selected geographical aspects of the Czech Republic, mainly as follows: (a) position in Europe, (b) geodiversity - evolution of natural environment, landscape types, (c) development of settlement, history and recent demographical trends, (d) economic significance, (e) cross-border relations, (f) environmental problems and (g) regional development issues. Students are attending consultations, where they get tasks and discussion questions for the above mentioned issues, and concurrently they work on a project covering these issues.</t>
+  </si>
+  <si>
     <t>Cílem předmětu je naučit se, jak sociobiologie v současné době umožňuje porozumět chování z evolučně biologického hlediska (v rozsahu knihy Alcock J. The Triumph of Sociobiology. New York: Oxford University Press 2003). Seznámíme se s kritikou, kterou tento postup původně vyvolal. Naučíme se základní terminologii používanou v této oblasti. Porozumíme základním principům chování a moderním sociobiologickým náhledům.</t>
-  </si>
-  <si>
-    <t>The course focuses on selected geographical aspects of the Czech Republic, mainly as follows: (a) position in Europe, (b) geodiversity - evolution of natural environment, landscape types, (c) development of settlement, history and recent demographical trends, (d) economic significance, (e) cross-border relations, (f) environmental problems and (g) regional development issues. Students are attending consultations, where they get tasks and discussion questions for the above mentioned issues, and concurrently they work on a project covering these issues.</t>
   </si>
   <si>
     <t>The course is designed for students of biological sciences. The aim of the course is to introduce students to the issues of microfluidic devices for analytical and bioanalytical purposes in the biological sciences.</t>
@@ -1924,10 +1924,10 @@
 </t>
   </si>
   <si>
+    <t>- hodnocení vedoucího diplomové práce</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prezentace referátů na cvičeních. </t>
-  </si>
-  <si>
-    <t>- hodnocení vedoucího diplomové práce</t>
   </si>
   <si>
     <t>Student vykonává přímou i nepřímou pedagogickou praxi na příslušném stupni školy dle pokynů Centra pro pedagogickou praxi: https://www.pf.ujep.cz/cpp/pokyny/ks</t>
@@ -6745,7 +6745,7 @@
     </row>
     <row r="25" spans="1:69">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>99</v>
@@ -6757,7 +6757,7 @@
         <v>171</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>226</v>
+        <v>171</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>235</v>
@@ -6766,16 +6766,20 @@
         <v>235</v>
       </c>
       <c r="H25" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>237</v>
       </c>
       <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+      <c r="K25" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>245</v>
+      </c>
       <c r="M25" s="1" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -6787,10 +6791,14 @@
       <c r="S25" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
+      <c r="T25" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>336</v>
+      </c>
       <c r="V25" s="1" t="s">
-        <v>289</v>
+        <v>337</v>
       </c>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -6799,36 +6807,30 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
-      <c r="AD25" s="1" t="s">
-        <v>370</v>
-      </c>
+      <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
-      <c r="AF25" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="AG25" s="1" t="s">
-        <v>404</v>
-      </c>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
       <c r="AH25" s="1" t="s">
         <v>236</v>
       </c>
       <c r="AI25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ25" s="1" t="s">
         <v>406</v>
       </c>
       <c r="AK25" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AL25" s="1" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="AM25" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN25" s="1" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="AO25" s="1" t="s">
         <v>427</v>
@@ -6837,23 +6839,17 @@
         <v>468</v>
       </c>
       <c r="AQ25" s="1" t="s">
-        <v>469</v>
+        <v>237</v>
       </c>
       <c r="AR25" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="AS25" s="1" t="s">
-        <v>485</v>
-      </c>
+      <c r="AS25" s="1"/>
       <c r="AT25" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="AU25" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="AV25" s="1" t="s">
-        <v>558</v>
-      </c>
+        <v>522</v>
+      </c>
+      <c r="AU25" s="1"/>
+      <c r="AV25" s="1"/>
       <c r="AW25" s="1"/>
       <c r="AX25" s="1"/>
       <c r="AY25" s="1" t="s">
@@ -6867,9 +6863,11 @@
         <v>236</v>
       </c>
       <c r="BC25" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="BD25" s="1"/>
+        <v>235</v>
+      </c>
+      <c r="BD25" s="1" t="s">
+        <v>565</v>
+      </c>
       <c r="BE25" s="1"/>
       <c r="BF25" s="1"/>
       <c r="BG25" s="1" t="s">
@@ -6896,7 +6894,7 @@
     </row>
     <row r="26" spans="1:69">
       <c r="A26" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>99</v>
@@ -6908,7 +6906,7 @@
         <v>172</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>172</v>
+        <v>226</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>235</v>
@@ -6917,20 +6915,16 @@
         <v>235</v>
       </c>
       <c r="H26" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>237</v>
       </c>
       <c r="J26" s="1"/>
-      <c r="K26" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>245</v>
-      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
       <c r="M26" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -6942,14 +6936,10 @@
       <c r="S26" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="T26" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="U26" s="1" t="s">
-        <v>336</v>
-      </c>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
       <c r="V26" s="1" t="s">
-        <v>337</v>
+        <v>289</v>
       </c>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
@@ -6958,30 +6948,36 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
-      <c r="AD26" s="1"/>
+      <c r="AD26" s="1" t="s">
+        <v>370</v>
+      </c>
       <c r="AE26" s="1"/>
-      <c r="AF26" s="1"/>
-      <c r="AG26" s="1"/>
+      <c r="AF26" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>404</v>
+      </c>
       <c r="AH26" s="1" t="s">
         <v>236</v>
       </c>
       <c r="AI26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ26" s="1" t="s">
         <v>406</v>
       </c>
       <c r="AK26" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AL26" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="AM26" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AN26" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="AO26" s="1" t="s">
         <v>428</v>
@@ -6990,17 +6986,23 @@
         <v>468</v>
       </c>
       <c r="AQ26" s="1" t="s">
-        <v>237</v>
+        <v>469</v>
       </c>
       <c r="AR26" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="AS26" s="1"/>
+      <c r="AS26" s="1" t="s">
+        <v>485</v>
+      </c>
       <c r="AT26" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="AU26" s="1"/>
-      <c r="AV26" s="1"/>
+        <v>523</v>
+      </c>
+      <c r="AU26" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="AV26" s="1" t="s">
+        <v>558</v>
+      </c>
       <c r="AW26" s="1"/>
       <c r="AX26" s="1"/>
       <c r="AY26" s="1" t="s">
@@ -7014,11 +7016,9 @@
         <v>236</v>
       </c>
       <c r="BC26" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="BD26" s="1" t="s">
-        <v>565</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="BD26" s="1"/>
       <c r="BE26" s="1"/>
       <c r="BF26" s="1"/>
       <c r="BG26" s="1" t="s">
@@ -7317,7 +7317,7 @@
     </row>
     <row r="29" spans="1:69">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>102</v>
@@ -7380,9 +7380,7 @@
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
-      <c r="AE29" s="1" t="s">
-        <v>400</v>
-      </c>
+      <c r="AE29" s="1"/>
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
       <c r="AH29" s="1" t="s">
@@ -7441,7 +7439,7 @@
       <c r="BE29" s="1"/>
       <c r="BF29" s="1"/>
       <c r="BG29" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="BH29" s="1" t="s">
         <v>236</v>
@@ -7451,9 +7449,7 @@
         <v>0</v>
       </c>
       <c r="BK29" s="1"/>
-      <c r="BL29" s="1" t="s">
-        <v>567</v>
-      </c>
+      <c r="BL29" s="1"/>
       <c r="BM29" s="1" t="s">
         <v>235</v>
       </c>
@@ -7466,7 +7462,7 @@
     </row>
     <row r="30" spans="1:69">
       <c r="A30" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>102</v>
@@ -7529,7 +7525,9 @@
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
-      <c r="AE30" s="1"/>
+      <c r="AE30" s="1" t="s">
+        <v>400</v>
+      </c>
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
       <c r="AH30" s="1" t="s">
@@ -7588,7 +7586,7 @@
       <c r="BE30" s="1"/>
       <c r="BF30" s="1"/>
       <c r="BG30" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="BH30" s="1" t="s">
         <v>236</v>
@@ -7598,7 +7596,9 @@
         <v>0</v>
       </c>
       <c r="BK30" s="1"/>
-      <c r="BL30" s="1"/>
+      <c r="BL30" s="1" t="s">
+        <v>567</v>
+      </c>
       <c r="BM30" s="1" t="s">
         <v>235</v>
       </c>
@@ -9536,7 +9536,7 @@
     </row>
     <row r="44" spans="1:69">
       <c r="A44" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>116</v>
@@ -9551,26 +9551,22 @@
         <v>229</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>235</v>
       </c>
       <c r="H44" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>237</v>
       </c>
       <c r="J44" s="1"/>
-      <c r="K44" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>281</v>
-      </c>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
       <c r="M44" s="1" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
@@ -9594,14 +9590,12 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
-      <c r="AD44" s="1" t="s">
-        <v>378</v>
-      </c>
+      <c r="AD44" s="1"/>
       <c r="AE44" s="1"/>
       <c r="AF44" s="1"/>
       <c r="AG44" s="1"/>
       <c r="AH44" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AI44" s="2">
         <v>0</v>
@@ -9610,7 +9604,7 @@
         <v>407</v>
       </c>
       <c r="AK44" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AL44" s="1" t="s">
         <v>407</v>
@@ -9621,24 +9615,18 @@
       <c r="AN44" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="AO44" s="1" t="s">
-        <v>440</v>
-      </c>
+      <c r="AO44" s="1"/>
       <c r="AP44" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AQ44" s="1" t="s">
-        <v>237</v>
+        <v>469</v>
       </c>
       <c r="AR44" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="AS44" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="AT44" s="1" t="s">
-        <v>533</v>
-      </c>
+      <c r="AS44" s="1"/>
+      <c r="AT44" s="1"/>
       <c r="AU44" s="1"/>
       <c r="AV44" s="1"/>
       <c r="AW44" s="1"/>
@@ -9663,7 +9651,7 @@
         <v>236</v>
       </c>
       <c r="BH44" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="BI44" s="1"/>
       <c r="BJ44" s="2">
@@ -9680,9 +9668,7 @@
         <v>289</v>
       </c>
       <c r="BO44" s="1"/>
-      <c r="BP44" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BP44" s="1"/>
       <c r="BQ44" s="1"/>
     </row>
     <row r="45" spans="1:69">
@@ -9696,10 +9682,10 @@
         <v>2023</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>235</v>
@@ -9836,7 +9822,7 @@
     </row>
     <row r="46" spans="1:69">
       <c r="A46" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>116</v>
@@ -9851,22 +9837,26 @@
         <v>230</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>235</v>
       </c>
       <c r="H46" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>237</v>
       </c>
       <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
+      <c r="K46" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="M46" s="1" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -9890,12 +9880,14 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
       <c r="AC46" s="1"/>
-      <c r="AD46" s="1"/>
+      <c r="AD46" s="1" t="s">
+        <v>378</v>
+      </c>
       <c r="AE46" s="1"/>
       <c r="AF46" s="1"/>
       <c r="AG46" s="1"/>
       <c r="AH46" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AI46" s="2">
         <v>0</v>
@@ -9904,7 +9896,7 @@
         <v>407</v>
       </c>
       <c r="AK46" s="2">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="AL46" s="1" t="s">
         <v>407</v>
@@ -9915,18 +9907,24 @@
       <c r="AN46" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="AO46" s="1"/>
+      <c r="AO46" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="AP46" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AQ46" s="1" t="s">
-        <v>469</v>
+        <v>237</v>
       </c>
       <c r="AR46" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="AS46" s="1"/>
-      <c r="AT46" s="1"/>
+      <c r="AS46" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="AT46" s="1" t="s">
+        <v>533</v>
+      </c>
       <c r="AU46" s="1"/>
       <c r="AV46" s="1"/>
       <c r="AW46" s="1"/>
@@ -9951,7 +9949,7 @@
         <v>236</v>
       </c>
       <c r="BH46" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="BI46" s="1"/>
       <c r="BJ46" s="2">
@@ -9968,7 +9966,9 @@
         <v>289</v>
       </c>
       <c r="BO46" s="1"/>
-      <c r="BP46" s="1"/>
+      <c r="BP46" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BQ46" s="1"/>
     </row>
     <row r="47" spans="1:69">
@@ -10124,7 +10124,7 @@
     </row>
     <row r="48" spans="1:69">
       <c r="A48" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>118</v>
@@ -10151,14 +10151,10 @@
         <v>237</v>
       </c>
       <c r="J48" s="1"/>
-      <c r="K48" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>277</v>
-      </c>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
       <c r="M48" s="1" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -10179,59 +10175,47 @@
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
-      <c r="AA48" s="1" t="s">
-        <v>344</v>
-      </c>
+      <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
-      <c r="AD48" s="1" t="s">
-        <v>380</v>
-      </c>
+      <c r="AD48" s="1"/>
       <c r="AE48" s="1"/>
       <c r="AF48" s="1"/>
       <c r="AG48" s="1"/>
       <c r="AH48" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AI48" s="2">
+        <v>12</v>
+      </c>
+      <c r="AJ48" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="AK48" s="2">
         <v>4</v>
       </c>
-      <c r="AJ48" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="AK48" s="2">
-        <v>5</v>
-      </c>
       <c r="AL48" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AM48" s="2">
         <v>0</v>
       </c>
       <c r="AN48" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="AO48" s="1" t="s">
-        <v>442</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="AO48" s="1"/>
       <c r="AP48" s="1" t="s">
         <v>468</v>
       </c>
       <c r="AQ48" s="1" t="s">
-        <v>237</v>
+        <v>469</v>
       </c>
       <c r="AR48" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="AS48" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="AT48" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="AU48" s="1" t="s">
-        <v>556</v>
-      </c>
+        <v>470</v>
+      </c>
+      <c r="AS48" s="1"/>
+      <c r="AT48" s="1"/>
+      <c r="AU48" s="1"/>
       <c r="AV48" s="1"/>
       <c r="AW48" s="1"/>
       <c r="AX48" s="1"/>
@@ -10255,15 +10239,17 @@
         <v>236</v>
       </c>
       <c r="BH48" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="BI48" s="1"/>
       <c r="BJ48" s="2">
         <v>0</v>
       </c>
-      <c r="BK48" s="1"/>
+      <c r="BK48" s="1" t="s">
+        <v>567</v>
+      </c>
       <c r="BL48" s="1" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="BM48" s="1" t="s">
         <v>235</v>
@@ -10277,7 +10263,7 @@
     </row>
     <row r="49" spans="1:69">
       <c r="A49" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>118</v>
@@ -10304,10 +10290,14 @@
         <v>237</v>
       </c>
       <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
+      <c r="K49" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="M49" s="1" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
@@ -10328,47 +10318,59 @@
       <c r="X49" s="1"/>
       <c r="Y49" s="1"/>
       <c r="Z49" s="1"/>
-      <c r="AA49" s="1"/>
+      <c r="AA49" s="1" t="s">
+        <v>344</v>
+      </c>
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
-      <c r="AD49" s="1"/>
+      <c r="AD49" s="1" t="s">
+        <v>380</v>
+      </c>
       <c r="AE49" s="1"/>
       <c r="AF49" s="1"/>
       <c r="AG49" s="1"/>
       <c r="AH49" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AI49" s="2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="AJ49" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AK49" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL49" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AM49" s="2">
         <v>0</v>
       </c>
       <c r="AN49" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="AO49" s="1"/>
+        <v>407</v>
+      </c>
+      <c r="AO49" s="1" t="s">
+        <v>442</v>
+      </c>
       <c r="AP49" s="1" t="s">
         <v>468</v>
       </c>
       <c r="AQ49" s="1" t="s">
-        <v>469</v>
+        <v>237</v>
       </c>
       <c r="AR49" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="AS49" s="1"/>
-      <c r="AT49" s="1"/>
-      <c r="AU49" s="1"/>
+        <v>471</v>
+      </c>
+      <c r="AS49" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="AT49" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="AU49" s="1" t="s">
+        <v>556</v>
+      </c>
       <c r="AV49" s="1"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
@@ -10392,17 +10394,15 @@
         <v>236</v>
       </c>
       <c r="BH49" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="BI49" s="1"/>
       <c r="BJ49" s="2">
         <v>0</v>
       </c>
-      <c r="BK49" s="1" t="s">
+      <c r="BK49" s="1"/>
+      <c r="BL49" s="1" t="s">
         <v>567</v>
-      </c>
-      <c r="BL49" s="1" t="s">
-        <v>569</v>
       </c>
       <c r="BM49" s="1" t="s">
         <v>235</v>
@@ -12327,7 +12327,7 @@
     </row>
     <row r="63" spans="1:69">
       <c r="A63" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>132</v>
@@ -12339,7 +12339,7 @@
         <v>203</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>236</v>
@@ -12348,20 +12348,16 @@
         <v>235</v>
       </c>
       <c r="H63" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>237</v>
       </c>
       <c r="J63" s="1"/>
-      <c r="K63" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>285</v>
-      </c>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
       <c r="M63" s="1" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
@@ -12386,7 +12382,7 @@
       <c r="AB63" s="1"/>
       <c r="AC63" s="1"/>
       <c r="AD63" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="AE63" s="1"/>
       <c r="AF63" s="1"/>
@@ -12401,7 +12397,7 @@
         <v>406</v>
       </c>
       <c r="AK63" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL63" s="1" t="s">
         <v>406</v>
@@ -12413,7 +12409,7 @@
         <v>406</v>
       </c>
       <c r="AO63" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="AP63" s="1" t="s">
         <v>467</v>
@@ -12427,9 +12423,7 @@
       <c r="AS63" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="AT63" s="1" t="s">
-        <v>545</v>
-      </c>
+      <c r="AT63" s="1"/>
       <c r="AU63" s="1"/>
       <c r="AV63" s="1"/>
       <c r="AW63" s="1"/>
@@ -12476,7 +12470,7 @@
     </row>
     <row r="64" spans="1:69">
       <c r="A64" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>132</v>
@@ -12488,7 +12482,7 @@
         <v>204</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>236</v>
@@ -12497,16 +12491,20 @@
         <v>235</v>
       </c>
       <c r="H64" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>237</v>
       </c>
       <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
+      <c r="K64" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="M64" s="1" t="s">
-        <v>289</v>
+        <v>313</v>
       </c>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
@@ -12531,7 +12529,7 @@
       <c r="AB64" s="1"/>
       <c r="AC64" s="1"/>
       <c r="AD64" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="AE64" s="1"/>
       <c r="AF64" s="1"/>
@@ -12546,7 +12544,7 @@
         <v>406</v>
       </c>
       <c r="AK64" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL64" s="1" t="s">
         <v>406</v>
@@ -12558,7 +12556,7 @@
         <v>406</v>
       </c>
       <c r="AO64" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="AP64" s="1" t="s">
         <v>467</v>
@@ -12572,7 +12570,9 @@
       <c r="AS64" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="AT64" s="1"/>
+      <c r="AT64" s="1" t="s">
+        <v>545</v>
+      </c>
       <c r="AU64" s="1"/>
       <c r="AV64" s="1"/>
       <c r="AW64" s="1"/>
@@ -13044,7 +13044,7 @@
     </row>
     <row r="68" spans="1:69">
       <c r="A68" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>135</v>
@@ -13053,10 +13053,10 @@
         <v>2023</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>235</v>
@@ -13065,20 +13065,20 @@
         <v>235</v>
       </c>
       <c r="H68" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>237</v>
       </c>
       <c r="J68" s="1"/>
       <c r="K68" s="1" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
@@ -13103,7 +13103,7 @@
       <c r="AB68" s="1"/>
       <c r="AC68" s="1"/>
       <c r="AD68" s="1" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="AE68" s="1"/>
       <c r="AF68" s="1"/>
@@ -13118,10 +13118,10 @@
         <v>406</v>
       </c>
       <c r="AK68" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL68" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AM68" s="2">
         <v>0</v>
@@ -13130,7 +13130,7 @@
         <v>406</v>
       </c>
       <c r="AO68" s="1" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
       <c r="AP68" s="1" t="s">
         <v>467</v>
@@ -13139,10 +13139,14 @@
         <v>237</v>
       </c>
       <c r="AR68" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="AS68" s="1"/>
-      <c r="AT68" s="1"/>
+        <v>472</v>
+      </c>
+      <c r="AS68" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="AT68" s="1" t="s">
+        <v>532</v>
+      </c>
       <c r="AU68" s="1"/>
       <c r="AV68" s="1"/>
       <c r="AW68" s="1"/>
@@ -13175,7 +13179,7 @@
       </c>
       <c r="BK68" s="1"/>
       <c r="BL68" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="BM68" s="1" t="s">
         <v>235</v>
@@ -13189,7 +13193,7 @@
     </row>
     <row r="69" spans="1:69">
       <c r="A69" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>135</v>
@@ -13198,10 +13202,10 @@
         <v>2023</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>235</v>
@@ -13210,20 +13214,20 @@
         <v>235</v>
       </c>
       <c r="H69" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>237</v>
       </c>
       <c r="J69" s="1"/>
       <c r="K69" s="1" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
@@ -13248,7 +13252,7 @@
       <c r="AB69" s="1"/>
       <c r="AC69" s="1"/>
       <c r="AD69" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="AE69" s="1"/>
       <c r="AF69" s="1"/>
@@ -13263,10 +13267,10 @@
         <v>406</v>
       </c>
       <c r="AK69" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL69" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AM69" s="2">
         <v>0</v>
@@ -13275,7 +13279,7 @@
         <v>406</v>
       </c>
       <c r="AO69" s="1" t="s">
-        <v>439</v>
+        <v>456</v>
       </c>
       <c r="AP69" s="1" t="s">
         <v>467</v>
@@ -13284,14 +13288,10 @@
         <v>237</v>
       </c>
       <c r="AR69" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="AS69" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="AT69" s="1" t="s">
-        <v>532</v>
-      </c>
+        <v>470</v>
+      </c>
+      <c r="AS69" s="1"/>
+      <c r="AT69" s="1"/>
       <c r="AU69" s="1"/>
       <c r="AV69" s="1"/>
       <c r="AW69" s="1"/>
@@ -13324,7 +13324,7 @@
       </c>
       <c r="BK69" s="1"/>
       <c r="BL69" s="1" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="BM69" s="1" t="s">
         <v>235</v>
@@ -15376,7 +15376,7 @@
     </row>
     <row r="84" spans="1:69">
       <c r="A84" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>150</v>
@@ -15431,13 +15431,11 @@
       <c r="AB84" s="1"/>
       <c r="AC84" s="1"/>
       <c r="AD84" s="1"/>
-      <c r="AE84" s="1" t="s">
-        <v>402</v>
-      </c>
+      <c r="AE84" s="1"/>
       <c r="AF84" s="1"/>
       <c r="AG84" s="1"/>
       <c r="AH84" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AI84" s="2">
         <v>0</v>
@@ -15457,7 +15455,9 @@
       <c r="AN84" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="AO84" s="1"/>
+      <c r="AO84" s="1" t="s">
+        <v>466</v>
+      </c>
       <c r="AP84" s="1" t="s">
         <v>468</v>
       </c>
@@ -15494,7 +15494,7 @@
         <v>566</v>
       </c>
       <c r="BG84" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="BH84" s="1" t="s">
         <v>236</v>
@@ -15509,9 +15509,7 @@
       <c r="BL84" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="BM84" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="BM84" s="1"/>
       <c r="BN84" s="1" t="s">
         <v>289</v>
       </c>
@@ -15521,7 +15519,7 @@
     </row>
     <row r="85" spans="1:69">
       <c r="A85" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>150</v>
@@ -15576,11 +15574,13 @@
       <c r="AB85" s="1"/>
       <c r="AC85" s="1"/>
       <c r="AD85" s="1"/>
-      <c r="AE85" s="1"/>
+      <c r="AE85" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="AF85" s="1"/>
       <c r="AG85" s="1"/>
       <c r="AH85" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AI85" s="2">
         <v>0</v>
@@ -15600,9 +15600,7 @@
       <c r="AN85" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="AO85" s="1" t="s">
-        <v>466</v>
-      </c>
+      <c r="AO85" s="1"/>
       <c r="AP85" s="1" t="s">
         <v>468</v>
       </c>
@@ -15639,7 +15637,7 @@
         <v>566</v>
       </c>
       <c r="BG85" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="BH85" s="1" t="s">
         <v>236</v>
@@ -15654,7 +15652,9 @@
       <c r="BL85" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="BM85" s="1"/>
+      <c r="BM85" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="BN85" s="1" t="s">
         <v>289</v>
       </c>

</xml_diff>